<commit_message>
Address lookup test data and locators fix done
</commit_message>
<xml_diff>
--- a/testData/Hana_T1002.xlsx
+++ b/testData/Hana_T1002.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C43969A-616E-4676-A17A-16F79A172241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57FB95B-A7A6-40A6-95EC-1E1AFD007A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>Flower Damaged</t>
   </si>
   <si>
-    <t>3286 B Hwy 100, Villa Ridge, MO 63089</t>
-  </si>
-  <si>
     <t>Alexandrianna</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>Starts At</t>
+  </si>
+  <si>
+    <t>3286b Hwy 100, Villa Ridge, MO 63089</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,22 +709,22 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>38</v>
@@ -736,10 +736,10 @@
         <v>39</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>40</v>

</xml_diff>